<commit_message>
fix(bar chart): remove jspdf
</commit_message>
<xml_diff>
--- a/public/Sample_template.xlsx
+++ b/public/Sample_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rahul\Desktop\office\infobell\project1\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28A654D0-8B48-4243-A183-222214ED4A46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E99DAEAE-D7AD-4B9D-BDBD-CFCCCDB0941D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{43F3C569-E911-4BC8-9EBC-874025E3B4E0}"/>
+    <workbookView xWindow="2580" yWindow="2580" windowWidth="19200" windowHeight="11170" xr2:uid="{43F3C569-E911-4BC8-9EBC-874025E3B4E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>uuid</t>
   </si>
@@ -81,15 +81,6 @@
   </si>
   <si>
     <t>spot</t>
-  </si>
-  <si>
-    <t>a9caea33-6afd-461d-a1df-7c095a247454</t>
-  </si>
-  <si>
-    <t>af-south-1</t>
-  </si>
-  <si>
-    <t>m7a.12xLarge</t>
   </si>
 </sst>
 </file>
@@ -500,7 +491,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -550,33 +541,8 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2">
-        <v>20</v>
-      </c>
-      <c r="F2">
-        <v>100</v>
-      </c>
-      <c r="G2">
-        <v>100</v>
-      </c>
-      <c r="H2">
-        <v>100</v>
-      </c>
-      <c r="I2">
-        <v>100</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="A2" s="4"/>
+      <c r="J2" s="3"/>
       <c r="L2" t="s">
         <v>10</v>
       </c>

</xml_diff>